<commit_message>
Фикс багов на : 1. Spec - special (((
</commit_message>
<xml_diff>
--- a/2.xlsx
+++ b/2.xlsx
@@ -717,6 +717,787 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>298</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="25" name="Image 25"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>313</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="26" name="Image 26"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>328</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="27" name="Image 27"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>343</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="28" name="Image 28"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>354</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="29" name="Image 29"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>365</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="30" name="Image 30"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>376</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="31" name="Image 31"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>387</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="32" name="Image 32"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>402</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="33" name="Image 33"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>413</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="34" name="Image 34"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>424</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="35" name="Image 35"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>435</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="36" name="Image 36"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>446</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="37" name="Image 37"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>461</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="38" name="Image 38"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>472</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="39" name="Image 39"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>487</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="40" name="Image 40"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>498</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="41" name="Image 41"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>509</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="42" name="Image 42"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>524</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="43" name="Image 43"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>535</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="44" name="Image 44"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>546</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="45" name="Image 45"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>561</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="46" name="Image 46"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>576</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="47" name="Image 47"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>591</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="48" name="Image 48"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>602</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="49" name="Image 49"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>617</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="50" name="Image 50"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>632</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="51" name="Image 51"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>643</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="52" name="Image 52"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId52"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1019,7 +1800,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AR285"/>
+  <dimension ref="A2:BF645"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1247,6 +2028,71 @@
           <t>Функция дозагрузки белья</t>
         </is>
       </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>Тип средства</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>Текстура</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>Объем</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>Тип кожи</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>Эффект</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>SPF-фактор</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>Особенности</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>Активные ингредиенты</t>
+        </is>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>Состав</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>Страна</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>Срок годности</t>
+        </is>
+      </c>
+      <c r="BD2" t="inlineStr">
+        <is>
+          <t>Масла и экстракты</t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>Дополнительная информация</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
@@ -2232,7 +3078,6 @@
           <t>нет</t>
         </is>
       </c>
-      <c r="AO285" t="inlineStr"/>
       <c r="AP285" t="inlineStr">
         <is>
           <t>пластик</t>
@@ -2246,6 +3091,892 @@
       <c r="AR285" t="inlineStr">
         <is>
           <t>через основной люк</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>BB крем Aspasia 4U SPF 50+/PA+++ 50ml</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--aspasia-bb-krem-4u-special-solution-spf-50-50-ml/651630186/spec</t>
+        </is>
+      </c>
+      <c r="AS300" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT300" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AU300" t="inlineStr">
+        <is>
+          <t>50 мл</t>
+        </is>
+      </c>
+      <c r="AV300" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная</t>
+        </is>
+      </c>
+      <c r="AW300" t="inlineStr">
+        <is>
+          <t>матирование, омоложение, отбеливание, увлажнение, защита от солнца</t>
+        </is>
+      </c>
+      <c r="AX300" t="inlineStr">
+        <is>
+          <t>SPF 50</t>
+        </is>
+      </c>
+      <c r="AY300" t="inlineStr">
+        <is>
+          <t>антивозрастной</t>
+        </is>
+      </c>
+      <c r="AZ300" t="inlineStr">
+        <is>
+          <t>глицерин</t>
+        </is>
+      </c>
+      <c r="BA300" t="inlineStr">
+        <is>
+          <t>очищенная вода, цетил этилгексаноат, диоксид титана, глицерин, минеральные масла, циклопентасилоксан, пэг/ппг-10/1 диметикон, сорбитансесквиолеат, пчелиный воск, хлорид натрия, диметикон/метилметикона кроссполимер, оксид цинка, триэтоксикаприлилсилан, феноксиэтанол, каприлил гликоль, экстракт риса, экстракт сосновой хвои, экстракт цветов лотоса, аллантоин, аденозин, дисодиум ЭДТА, желтый оксид железа, красный оксид железа, черный оксид железа, отдушка</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>BB крем Aspasia 4U SPF 50+/PA+++ 50ml</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--aspasia-bb-krem-4u-special-solution-spf-50-50-ml/651630186/spec</t>
+        </is>
+      </c>
+      <c r="AS315" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT315" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AU315" t="inlineStr">
+        <is>
+          <t>50 мл</t>
+        </is>
+      </c>
+      <c r="AV315" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная</t>
+        </is>
+      </c>
+      <c r="AW315" t="inlineStr">
+        <is>
+          <t>матирование, омоложение, отбеливание, увлажнение, защита от солнца</t>
+        </is>
+      </c>
+      <c r="AX315" t="inlineStr">
+        <is>
+          <t>SPF 50</t>
+        </is>
+      </c>
+      <c r="AY315" t="inlineStr">
+        <is>
+          <t>антивозрастной</t>
+        </is>
+      </c>
+      <c r="AZ315" t="inlineStr">
+        <is>
+          <t>глицерин</t>
+        </is>
+      </c>
+      <c r="BA315" t="inlineStr">
+        <is>
+          <t>очищенная вода, цетил этилгексаноат, диоксид титана, глицерин, минеральные масла, циклопентасилоксан, пэг/ппг-10/1 диметикон, сорбитансесквиолеат, пчелиный воск, хлорид натрия, диметикон/метилметикона кроссполимер, оксид цинка, триэтоксикаприлилсилан, феноксиэтанол, каприлил гликоль, экстракт риса, экстракт сосновой хвои, экстракт цветов лотоса, аллантоин, аденозин, дисодиум ЭДТА, желтый оксид железа, красный оксид железа, черный оксид железа, отдушка</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>BB крем Aspasia 4U Wrinkle 50ml</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--aspasia-bb-krem-4u-wrinkle-50-ml/653543044/spec</t>
+        </is>
+      </c>
+      <c r="AS330" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT330" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AU330" t="inlineStr">
+        <is>
+          <t>50 мл</t>
+        </is>
+      </c>
+      <c r="AV330" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная</t>
+        </is>
+      </c>
+      <c r="AW330" t="inlineStr">
+        <is>
+          <t>разглаживание морщин, отбеливание, увлажнение, маскировка несовершенств</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>BB крем Elizavecca Milky Piggy SPF50</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--elizavecca-bb-krem-milky-piggy-spf-50-50-ml/1946995634/spec</t>
+        </is>
+      </c>
+      <c r="AS345" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT345" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AU345" t="inlineStr">
+        <is>
+          <t>50 мл</t>
+        </is>
+      </c>
+      <c r="AV345" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная, проблемная</t>
+        </is>
+      </c>
+      <c r="AW345" t="inlineStr">
+        <is>
+          <t>восстановление, разглаживание морщин, отбеливание, увлажнение, тонирование, защита от солнца, лифтинг</t>
+        </is>
+      </c>
+      <c r="AX345" t="inlineStr">
+        <is>
+          <t>SPF 50</t>
+        </is>
+      </c>
+      <c r="AZ345" t="inlineStr">
+        <is>
+          <t>гиалуроновая кислота, коллаген</t>
+        </is>
+      </c>
+      <c r="BA345" t="inlineStr">
+        <is>
+          <t>water, titanium dioxide, ethylhexyl methoxycinnamate, phenyl trimethicone, glycerin, ethylhexyl salicylate, synthetic fluorphlogopite, ethylhexyl methoxycrylene , butyloctyl salicylate, triethylhexanoin, disteardimonium hectorite, propylene carbonate, butylene glycol, cetyl peg/ppg-10/1 dimethiconevp/hexadecene copolymer, niacinamide , butyl methoxydibenzoylmethane, sorbitan sesquioleate, sorbitan olivate, zinc stearate, triethanolamine, magnesium sulfate, sodium hyaluronate, ci 77492, caprylhydroxamic acid, caprylyl glycol, glycerin, ci 77499 , ci 77491, ceresin, phenoxyethanol, tocopheryl acetate, allantoin, panthenol, fragrance, water, glycerin, psidium guajava leaf extract, artemisia princeps extract, morus alba leaf extract, vitis vinifera (grape) seed extract , hydrolyzed collagen , disodium edta, adenosine</t>
+        </is>
+      </c>
+      <c r="BB345" t="inlineStr">
+        <is>
+          <t>Корея</t>
+        </is>
+      </c>
+      <c r="BC345" t="inlineStr">
+        <is>
+          <t>36 мес.</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>BB крем Farmstay Formula All-in-one Snail Sun BB Cream 50g</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--farmstay-formula-all-in-one-bb-krem-snail-sun-bb-cream-50-gr/1919506871/spec</t>
+        </is>
+      </c>
+      <c r="AK404" t="inlineStr">
+        <is>
+          <t>50 г</t>
+        </is>
+      </c>
+      <c r="AS404" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT404" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AV404" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная, проблемная</t>
+        </is>
+      </c>
+      <c r="AW404" t="inlineStr">
+        <is>
+          <t>восстановление, разглаживание морщин, отбеливание, питание, снятие воспалений, увлажнение, тонирование, защита от солнца, лифтинг</t>
+        </is>
+      </c>
+      <c r="AX404" t="inlineStr">
+        <is>
+          <t>SPF 50</t>
+        </is>
+      </c>
+      <c r="AZ404" t="inlineStr">
+        <is>
+          <t>витамины группы B, гиалуроновая кислота, муцин улитки</t>
+        </is>
+      </c>
+      <c r="BA404" t="inlineStr">
+        <is>
+          <t>aqua, ethylhexyl methoxycinnamate, titanium dioxide, zinc oxide, propylene glycol, paraffinum liquidum, cyclomethicone, butylene glycol, niacinamide, cetyl peg/ppg-10/1dimethicone, dimethicone, caprylic/capric triglyceride, glycerin, olea europaea (olive) fruit oil, zinc stearate, hyaluronic acid, sorbitan sesquioleate, cl 77491, cl 77499, beeswax, methylparaben, propylparaben, adenosine, disodium edta, flavor, cl 77492</t>
+        </is>
+      </c>
+      <c r="BB404" t="inlineStr">
+        <is>
+          <t>Корея</t>
+        </is>
+      </c>
+      <c r="BC404" t="inlineStr">
+        <is>
+          <t>12 мес.</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>BB крем Farmstay Зеленый чай 50мл</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--farmstay-bb-krem-pure-anti-wrinkle-green-tea-seed-40-g/1919506790/spec</t>
+        </is>
+      </c>
+      <c r="AK463" t="inlineStr">
+        <is>
+          <t>40 г</t>
+        </is>
+      </c>
+      <c r="AS463" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT463" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AV463" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная, проблемная</t>
+        </is>
+      </c>
+      <c r="AW463" t="inlineStr">
+        <is>
+          <t>матирование, разглаживание морщин, питание, увлажнение, тонирование, лифтинг</t>
+        </is>
+      </c>
+      <c r="AY463" t="inlineStr">
+        <is>
+          <t>антивозрастной</t>
+        </is>
+      </c>
+      <c r="AZ463" t="inlineStr">
+        <is>
+          <t>гиалуроновая кислота</t>
+        </is>
+      </c>
+      <c r="BB463" t="inlineStr">
+        <is>
+          <t>Корея</t>
+        </is>
+      </c>
+      <c r="BC463" t="inlineStr">
+        <is>
+          <t>12 мес.</t>
+        </is>
+      </c>
+      <c r="BD463" t="inlineStr">
+        <is>
+          <t>экстракт алоэ, экстракт зеленого чая</t>
+        </is>
+      </c>
+      <c r="BE463" t="inlineStr">
+        <is>
+          <t>содержит экстракт жасмина, аденозин</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>BB крем Farmstay Королевская Улитка</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--farmstay-bb-krem-noblesse-intensive-escargot-spf-48-50-g/1919466676/spec</t>
+        </is>
+      </c>
+      <c r="AK489" t="inlineStr">
+        <is>
+          <t>50 г</t>
+        </is>
+      </c>
+      <c r="AS489" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT489" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AV489" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная, проблемная</t>
+        </is>
+      </c>
+      <c r="AW489" t="inlineStr">
+        <is>
+          <t>восстановление, матирование, разглаживание морщин, отбеливание, питание, снятие воспалений, увлажнение, тонирование, защита от солнца, лифтинг</t>
+        </is>
+      </c>
+      <c r="AX489" t="inlineStr">
+        <is>
+          <t>SPF 48</t>
+        </is>
+      </c>
+      <c r="AY489" t="inlineStr">
+        <is>
+          <t>антивозрастной</t>
+        </is>
+      </c>
+      <c r="AZ489" t="inlineStr">
+        <is>
+          <t>витамин А, витамин Е, витамины группы B, гиалуроновая кислота, коллаген, муцин улитки</t>
+        </is>
+      </c>
+      <c r="BA489" t="inlineStr">
+        <is>
+          <t>water, cyclopentasiloxane, cyclohexasiloxane, titanium dioxide, glycerin, dimethicone, sodium hyaluronate niacinamide, lilium tigrinum extract, aloe barbadensis leaf extract, lavandula angustifolia (lavender) extract, magnolia kobus bark extract, phenoxyethanol, aluminum hydroxide, stearic acid, peg-10 dimethicone, methylparaben, propylparaben, xanthan gum, allantoin, disodium edta, snail secretion filtrate, perfume</t>
+        </is>
+      </c>
+      <c r="BB489" t="inlineStr">
+        <is>
+          <t>Корея</t>
+        </is>
+      </c>
+      <c r="BC489" t="inlineStr">
+        <is>
+          <t>365 дн.</t>
+        </is>
+      </c>
+      <c r="BD489" t="inlineStr">
+        <is>
+          <t>экстракт алоэ</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>BB крем Farmstay Улитка SPF +50</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--farmstay-bb-krem-snail-repair-formula-all-in-one-spf-50-50-g/1919466678/spec</t>
+        </is>
+      </c>
+      <c r="AK526" t="inlineStr">
+        <is>
+          <t>50 г</t>
+        </is>
+      </c>
+      <c r="AS526" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT526" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AV526" t="inlineStr">
+        <is>
+          <t>жирная, комбинированная, нормальная</t>
+        </is>
+      </c>
+      <c r="AW526" t="inlineStr">
+        <is>
+          <t>восстановление, разглаживание морщин, отбеливание, питание, снятие воспалений, сужение пор, увлажнение, тонирование, защита от солнца, лифтинг</t>
+        </is>
+      </c>
+      <c r="AX526" t="inlineStr">
+        <is>
+          <t>SPF 50</t>
+        </is>
+      </c>
+      <c r="AZ526" t="inlineStr">
+        <is>
+          <t>витамины группы B, гиалуроновая кислота, муцин улитки, пантенол</t>
+        </is>
+      </c>
+      <c r="BA526" t="inlineStr">
+        <is>
+          <t>water, titanium dioxide /trimethoxycaprylylsilane, ethylhexyl methoxycinnamate, zinc oxide, mineral oil, paraffinum liquidum, cyclomethicone, butyl methoxydibenzoylmethane, caprylic/capric triglyceride, butylene glycol, niacinamide, propylene glycol, glycerine, cetyl peg/ppg-10/1 dimethicone, sorbitan sesquioleate, butyrospermum parkii (shea) butter, sodium chloride, bees wax, sodium hyaluronate, microcrystalline wax, aloe barbadenis leaf extract, hamamelis virginiana (witch hazel) extract, chamomilla recutita (matricaria) extract, camellia sinensis leaf extract, centella asiatica extract, rose centifolia flower water, collagen extract, snail secretion filtrate, adenosine, propylparaben, methylparaben, ci 77491, ci 77492, ci 77499, fragrance</t>
+        </is>
+      </c>
+      <c r="BB526" t="inlineStr">
+        <is>
+          <t>Корея</t>
+        </is>
+      </c>
+      <c r="BC526" t="inlineStr">
+        <is>
+          <t>12 мес.</t>
+        </is>
+      </c>
+      <c r="BE526" t="inlineStr">
+        <is>
+          <t>содержит арбутин, аллантоин, аденозин, экстракт полыни, папайи, тысячелистника, арники</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>BB крем Aspasia 4U SPF 50+/PA+++ 50ml</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--aspasia-bb-krem-4u-special-solution-spf-50-50-ml/651630186/spec</t>
+        </is>
+      </c>
+      <c r="AS563" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT563" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AU563" t="inlineStr">
+        <is>
+          <t>50 мл</t>
+        </is>
+      </c>
+      <c r="AV563" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная</t>
+        </is>
+      </c>
+      <c r="AW563" t="inlineStr">
+        <is>
+          <t>матирование, омоложение, отбеливание, увлажнение, защита от солнца</t>
+        </is>
+      </c>
+      <c r="AX563" t="inlineStr">
+        <is>
+          <t>SPF 50</t>
+        </is>
+      </c>
+      <c r="AY563" t="inlineStr">
+        <is>
+          <t>антивозрастной</t>
+        </is>
+      </c>
+      <c r="AZ563" t="inlineStr">
+        <is>
+          <t>глицерин</t>
+        </is>
+      </c>
+      <c r="BA563" t="inlineStr">
+        <is>
+          <t>очищенная вода, цетил этилгексаноат, диоксид титана, глицерин, минеральные масла, циклопентасилоксан, пэг/ппг-10/1 диметикон, сорбитансесквиолеат, пчелиный воск, хлорид натрия, диметикон/метилметикона кроссполимер, оксид цинка, триэтоксикаприлилсилан, феноксиэтанол, каприлил гликоль, экстракт риса, экстракт сосновой хвои, экстракт цветов лотоса, аллантоин, аденозин, дисодиум ЭДТА, желтый оксид железа, красный оксид железа, черный оксид железа, отдушка</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>BB крем Aspasia 4U Wrinkle 50ml</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--aspasia-bb-krem-4u-wrinkle-50-ml/653543044/spec</t>
+        </is>
+      </c>
+      <c r="AS578" t="inlineStr">
+        <is>
+          <t>BB крем</t>
+        </is>
+      </c>
+      <c r="AT578" t="inlineStr">
+        <is>
+          <t>кремовая</t>
+        </is>
+      </c>
+      <c r="AU578" t="inlineStr">
+        <is>
+          <t>50 мл</t>
+        </is>
+      </c>
+      <c r="AV578" t="inlineStr">
+        <is>
+          <t>для всех типов, жирная, комбинированная, сухая, нормальная, чувствительная</t>
+        </is>
+      </c>
+      <c r="AW578" t="inlineStr">
+        <is>
+          <t>разглаживание морщин, отбеливание, увлажнение, маскировка несовершенств</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Стиральная машина Artel TE 60 L</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--stiralnaia-mashina-artel-te60l/13802748/spec</t>
+        </is>
+      </c>
+      <c r="AD593" t="inlineStr">
+        <is>
+          <t>да</t>
+        </is>
+      </c>
+      <c r="AE593" t="inlineStr">
+        <is>
+          <t>отдельно стоящая</t>
+        </is>
+      </c>
+      <c r="AF593" t="inlineStr">
+        <is>
+          <t>вертикальная</t>
+        </is>
+      </c>
+      <c r="AG593" t="inlineStr">
+        <is>
+          <t>6 кг</t>
+        </is>
+      </c>
+      <c r="AH593" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AI593" t="inlineStr">
+        <is>
+          <t>механическое</t>
+        </is>
+      </c>
+      <c r="AJ593" t="inlineStr">
+        <is>
+          <t>74x44x85 см</t>
+        </is>
+      </c>
+      <c r="AK593" t="inlineStr">
+        <is>
+          <t>19 кг</t>
+        </is>
+      </c>
+      <c r="AL593" t="inlineStr">
+        <is>
+          <t>серый</t>
+        </is>
+      </c>
+      <c r="AM593" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AN593" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AP593" t="inlineStr">
+        <is>
+          <t>пластик</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Стиральная машина Artel TG 100 FP</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--stiralnaia-mashina-artel-tg100fp-red/217193208/spec</t>
+        </is>
+      </c>
+      <c r="AD619" t="inlineStr">
+        <is>
+          <t>да</t>
+        </is>
+      </c>
+      <c r="AE619" t="inlineStr">
+        <is>
+          <t>отдельно стоящая</t>
+        </is>
+      </c>
+      <c r="AF619" t="inlineStr">
+        <is>
+          <t>вертикальная</t>
+        </is>
+      </c>
+      <c r="AG619" t="inlineStr">
+        <is>
+          <t>10 кг</t>
+        </is>
+      </c>
+      <c r="AH619" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AI619" t="inlineStr">
+        <is>
+          <t>механическое</t>
+        </is>
+      </c>
+      <c r="AJ619" t="inlineStr">
+        <is>
+          <t>85x51x96 см</t>
+        </is>
+      </c>
+      <c r="AK619" t="inlineStr">
+        <is>
+          <t>30.5 кг</t>
+        </is>
+      </c>
+      <c r="AL619" t="inlineStr">
+        <is>
+          <t>белый</t>
+        </is>
+      </c>
+      <c r="AM619" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AN619" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AP619" t="inlineStr">
+        <is>
+          <t>пластик</t>
+        </is>
+      </c>
+      <c r="AQ619" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AR619" t="inlineStr">
+        <is>
+          <t>через основной люк</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Стиральная машина Artel TG 101 FP</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://market.yandex.kz/product--stiralnaia-mashina-artel-tg101fp-blue/1968870507/spec</t>
+        </is>
+      </c>
+      <c r="AD634" t="inlineStr">
+        <is>
+          <t>да</t>
+        </is>
+      </c>
+      <c r="AE634" t="inlineStr">
+        <is>
+          <t>отдельно стоящая</t>
+        </is>
+      </c>
+      <c r="AF634" t="inlineStr">
+        <is>
+          <t>вертикальная</t>
+        </is>
+      </c>
+      <c r="AG634" t="inlineStr">
+        <is>
+          <t>10 кг</t>
+        </is>
+      </c>
+      <c r="AH634" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AI634" t="inlineStr">
+        <is>
+          <t>механическое</t>
+        </is>
+      </c>
+      <c r="AJ634" t="inlineStr">
+        <is>
+          <t>85x51x97 см</t>
+        </is>
+      </c>
+      <c r="AK634" t="inlineStr">
+        <is>
+          <t>19 кг</t>
+        </is>
+      </c>
+      <c r="AL634" t="inlineStr">
+        <is>
+          <t>белый</t>
+        </is>
+      </c>
+      <c r="AM634" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AN634" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+      <c r="AO634" t="inlineStr"/>
+      <c r="AP634" t="inlineStr">
+        <is>
+          <t>пластик</t>
+        </is>
+      </c>
+      <c r="AR634" t="inlineStr">
+        <is>
+          <t>через основной люк</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>Максимальная строка</t>
         </is>
       </c>
     </row>

</xml_diff>